<commit_message>
trains holding authorities currently
</commit_message>
<xml_diff>
--- a/Schedule v4.xlsx
+++ b/Schedule v4.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\japro\OneDrive\Documents2\Pitt\Systems &amp; Project Engineering\2024 Fall Term\Lectures\Lecture 2 - Project\Project Information\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Trains C\trains\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F6FCB0A-0C47-4E7F-B20A-19A810E5CFED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCCE79B2-44AA-4F82-A752-2F70EA6610C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-5800" yWindow="-21710" windowWidth="38620" windowHeight="21220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Green Line Schedule" sheetId="7" r:id="rId1"/>
@@ -338,8 +338,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="0.0"/>
-    <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -451,7 +451,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -460,22 +460,22 @@
     <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="20" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="20" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -784,36 +784,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AQ163"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AF1" sqref="AF1:AQ1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.796875" style="3"/>
-    <col min="2" max="2" width="12.796875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="8.46484375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="11" style="3" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="10.53125" style="3" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="13.265625" style="3" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="35.9296875" style="3" customWidth="1"/>
-    <col min="8" max="12" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="11.46484375" style="1" hidden="1" customWidth="1"/>
-    <col min="14" max="17" width="8.796875" style="1" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="4.53125" style="1" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="3.53125" style="1" hidden="1" customWidth="1"/>
-    <col min="20" max="23" width="8.796875" style="1" hidden="1" customWidth="1"/>
-    <col min="24" max="24" width="19.265625" style="1" hidden="1" customWidth="1"/>
-    <col min="25" max="28" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="29" max="29" width="11.796875" style="1" hidden="1" customWidth="1"/>
-    <col min="30" max="31" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="32" max="36" width="10.73046875" style="22" customWidth="1"/>
-    <col min="37" max="41" width="8.796875" style="3"/>
-    <col min="42" max="42" width="4.46484375" style="1" customWidth="1"/>
-    <col min="43" max="16384" width="8.796875" style="1"/>
+    <col min="1" max="1" width="8.77734375" style="3"/>
+    <col min="2" max="2" width="12.77734375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="8.44140625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="11" style="3" customWidth="1"/>
+    <col min="5" max="5" width="10.5546875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="13.21875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="35.88671875" style="3" customWidth="1"/>
+    <col min="8" max="12" width="8.77734375" style="1" customWidth="1"/>
+    <col min="13" max="13" width="11.44140625" style="1" customWidth="1"/>
+    <col min="14" max="17" width="8.77734375" style="1" customWidth="1"/>
+    <col min="18" max="18" width="4.5546875" style="1" customWidth="1"/>
+    <col min="19" max="19" width="3.5546875" style="1" customWidth="1"/>
+    <col min="20" max="23" width="8.77734375" style="1" customWidth="1"/>
+    <col min="24" max="24" width="19.21875" style="1" customWidth="1"/>
+    <col min="25" max="28" width="8.77734375" style="1" customWidth="1"/>
+    <col min="29" max="29" width="11.77734375" style="1" customWidth="1"/>
+    <col min="30" max="31" width="8.77734375" style="1" customWidth="1"/>
+    <col min="32" max="36" width="10.77734375" style="22" customWidth="1"/>
+    <col min="37" max="41" width="8.77734375" style="3"/>
+    <col min="42" max="42" width="4.44140625" style="1" customWidth="1"/>
+    <col min="43" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" ht="37.9" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:43" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -933,7 +933,7 @@
         <v>2.0833333333333333E-3</v>
       </c>
     </row>
-    <row r="2" spans="1:43" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -1020,7 +1020,7 @@
         <v>1.8749999999999999E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:43" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="str">
         <f>A2</f>
         <v>Green</v>
@@ -1131,7 +1131,7 @@
         <v>4.8611111111111112E-3</v>
       </c>
       <c r="AI3" s="21">
-        <f t="shared" ref="AG3:AO3" si="6">AH3+$AQ$1</f>
+        <f t="shared" ref="AI3:AO3" si="6">AH3+$AQ$1</f>
         <v>6.9444444444444441E-3</v>
       </c>
       <c r="AJ3" s="21">
@@ -1159,7 +1159,7 @@
         <v>1.9444444444444441E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:43" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="str">
         <f t="shared" ref="A4:A67" si="7">A3</f>
         <v>Green</v>
@@ -1211,7 +1211,7 @@
       <c r="AI4" s="3"/>
       <c r="AJ4" s="3"/>
     </row>
-    <row r="5" spans="1:43" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -1263,7 +1263,7 @@
       <c r="AI5" s="3"/>
       <c r="AJ5" s="3"/>
     </row>
-    <row r="6" spans="1:43" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -1315,7 +1315,7 @@
       <c r="AI6" s="3"/>
       <c r="AJ6" s="3"/>
     </row>
-    <row r="7" spans="1:43" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -1367,7 +1367,7 @@
       <c r="AI7" s="3"/>
       <c r="AJ7" s="3"/>
     </row>
-    <row r="8" spans="1:43" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -1420,7 +1420,7 @@
       <c r="AI8" s="3"/>
       <c r="AJ8" s="3"/>
     </row>
-    <row r="9" spans="1:43" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -1472,7 +1472,7 @@
       <c r="AI9" s="3"/>
       <c r="AJ9" s="3"/>
     </row>
-    <row r="10" spans="1:43" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -1610,7 +1610,7 @@
         <v>2.1527777777777774E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:43" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -1660,7 +1660,7 @@
       <c r="AI11" s="3"/>
       <c r="AJ11" s="3"/>
     </row>
-    <row r="12" spans="1:43" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -1710,7 +1710,7 @@
       <c r="AI12" s="3"/>
       <c r="AJ12" s="3"/>
     </row>
-    <row r="13" spans="1:43" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -1763,7 +1763,7 @@
       <c r="AI13" s="3"/>
       <c r="AJ13" s="3"/>
     </row>
-    <row r="14" spans="1:43" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -1813,7 +1813,7 @@
       <c r="AI14" s="3"/>
       <c r="AJ14" s="3"/>
     </row>
-    <row r="15" spans="1:43" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -1863,7 +1863,7 @@
       <c r="AI15" s="3"/>
       <c r="AJ15" s="3"/>
     </row>
-    <row r="16" spans="1:43" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -1913,7 +1913,7 @@
       <c r="AI16" s="3"/>
       <c r="AJ16" s="3"/>
     </row>
-    <row r="17" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -2051,7 +2051,7 @@
         <v>2.4305555555555552E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -2101,7 +2101,7 @@
       <c r="AI18" s="3"/>
       <c r="AJ18" s="3"/>
     </row>
-    <row r="19" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -2151,7 +2151,7 @@
       <c r="AI19" s="3"/>
       <c r="AJ19" s="3"/>
     </row>
-    <row r="20" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -2201,7 +2201,7 @@
       <c r="AI20" s="3"/>
       <c r="AJ20" s="3"/>
     </row>
-    <row r="21" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -2251,7 +2251,7 @@
       <c r="AI21" s="3"/>
       <c r="AJ21" s="3"/>
     </row>
-    <row r="22" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -2301,7 +2301,7 @@
       <c r="AI22" s="3"/>
       <c r="AJ22" s="3"/>
     </row>
-    <row r="23" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -2439,7 +2439,7 @@
         <v>2.7083333333333331E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -2489,7 +2489,7 @@
       <c r="AI24" s="3"/>
       <c r="AJ24" s="3"/>
     </row>
-    <row r="25" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -2539,7 +2539,7 @@
       <c r="AI25" s="3"/>
       <c r="AJ25" s="3"/>
     </row>
-    <row r="26" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -2589,7 +2589,7 @@
       <c r="AI26" s="3"/>
       <c r="AJ26" s="3"/>
     </row>
-    <row r="27" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -2639,7 +2639,7 @@
       <c r="AI27" s="3"/>
       <c r="AJ27" s="3"/>
     </row>
-    <row r="28" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -2689,7 +2689,7 @@
       <c r="AI28" s="3"/>
       <c r="AJ28" s="3"/>
     </row>
-    <row r="29" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -2739,7 +2739,7 @@
       <c r="AI29" s="3"/>
       <c r="AJ29" s="3"/>
     </row>
-    <row r="30" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -2792,7 +2792,7 @@
       <c r="AI30" s="3"/>
       <c r="AJ30" s="3"/>
     </row>
-    <row r="31" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -2842,7 +2842,7 @@
       <c r="AI31" s="3"/>
       <c r="AJ31" s="3"/>
     </row>
-    <row r="32" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -2980,7 +2980,7 @@
         <v>2.9861111111111109E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -3030,7 +3030,7 @@
       <c r="AI33" s="3"/>
       <c r="AJ33" s="3"/>
     </row>
-    <row r="34" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -3080,7 +3080,7 @@
       <c r="AI34" s="3"/>
       <c r="AJ34" s="3"/>
     </row>
-    <row r="35" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -3130,7 +3130,7 @@
       <c r="AI35" s="3"/>
       <c r="AJ35" s="3"/>
     </row>
-    <row r="36" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -3180,7 +3180,7 @@
       <c r="AI36" s="3"/>
       <c r="AJ36" s="3"/>
     </row>
-    <row r="37" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -3233,7 +3233,7 @@
       <c r="AI37" s="3"/>
       <c r="AJ37" s="3"/>
     </row>
-    <row r="38" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="str">
         <f>A34</f>
         <v>Green</v>
@@ -3286,7 +3286,7 @@
       <c r="AI38" s="3"/>
       <c r="AJ38" s="3"/>
     </row>
-    <row r="39" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="39" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -3339,7 +3339,7 @@
       <c r="AI39" s="3"/>
       <c r="AJ39" s="3"/>
     </row>
-    <row r="40" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="40" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -3476,7 +3476,7 @@
         <v>3.1944444444444442E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="41" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -3529,7 +3529,7 @@
       <c r="AI41" s="3"/>
       <c r="AJ41" s="3"/>
     </row>
-    <row r="42" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="42" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -3582,7 +3582,7 @@
       <c r="AI42" s="3"/>
       <c r="AJ42" s="3"/>
     </row>
-    <row r="43" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="43" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -3635,7 +3635,7 @@
       <c r="AI43" s="3"/>
       <c r="AJ43" s="3"/>
     </row>
-    <row r="44" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="44" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -3688,7 +3688,7 @@
       <c r="AI44" s="3"/>
       <c r="AJ44" s="3"/>
     </row>
-    <row r="45" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="45" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -3741,7 +3741,7 @@
       <c r="AI45" s="3"/>
       <c r="AJ45" s="3"/>
     </row>
-    <row r="46" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="46" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -3794,7 +3794,7 @@
       <c r="AI46" s="3"/>
       <c r="AJ46" s="3"/>
     </row>
-    <row r="47" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="47" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -3847,7 +3847,7 @@
       <c r="AI47" s="3"/>
       <c r="AJ47" s="3"/>
     </row>
-    <row r="48" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="48" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -3900,7 +3900,7 @@
       <c r="AI48" s="3"/>
       <c r="AJ48" s="3"/>
     </row>
-    <row r="49" spans="1:41" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="49" spans="1:41" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -4037,7 +4037,7 @@
         <v>3.3333333333333333E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="50" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -4090,7 +4090,7 @@
       <c r="AI50" s="3"/>
       <c r="AJ50" s="3"/>
     </row>
-    <row r="51" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="51" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -4143,7 +4143,7 @@
       <c r="AI51" s="3"/>
       <c r="AJ51" s="3"/>
     </row>
-    <row r="52" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="52" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -4196,7 +4196,7 @@
       <c r="AI52" s="3"/>
       <c r="AJ52" s="3"/>
     </row>
-    <row r="53" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="53" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -4249,7 +4249,7 @@
       <c r="AI53" s="3"/>
       <c r="AJ53" s="3"/>
     </row>
-    <row r="54" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="54" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -4302,7 +4302,7 @@
       <c r="AI54" s="3"/>
       <c r="AJ54" s="3"/>
     </row>
-    <row r="55" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="55" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -4355,7 +4355,7 @@
       <c r="AI55" s="3"/>
       <c r="AJ55" s="3"/>
     </row>
-    <row r="56" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="56" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -4408,7 +4408,7 @@
       <c r="AI56" s="3"/>
       <c r="AJ56" s="3"/>
     </row>
-    <row r="57" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="57" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -4461,7 +4461,7 @@
       <c r="AI57" s="3"/>
       <c r="AJ57" s="3"/>
     </row>
-    <row r="58" spans="1:41" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="58" spans="1:41" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -4598,7 +4598,7 @@
         <v>3.5416666666666666E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="59" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -4651,7 +4651,7 @@
       <c r="AI59" s="3"/>
       <c r="AJ59" s="3"/>
     </row>
-    <row r="60" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="60" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -4701,7 +4701,7 @@
       <c r="AI60" s="3"/>
       <c r="AJ60" s="3"/>
     </row>
-    <row r="61" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="61" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -4751,7 +4751,7 @@
       <c r="AI61" s="3"/>
       <c r="AJ61" s="3"/>
     </row>
-    <row r="62" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="62" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A62" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -4801,7 +4801,7 @@
       <c r="AI62" s="3"/>
       <c r="AJ62" s="3"/>
     </row>
-    <row r="63" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="63" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -4854,7 +4854,7 @@
       <c r="AI63" s="3"/>
       <c r="AJ63" s="3"/>
     </row>
-    <row r="64" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="64" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A64" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -4904,7 +4904,7 @@
       <c r="AI64" s="3"/>
       <c r="AJ64" s="3"/>
     </row>
-    <row r="65" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="65" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -4954,7 +4954,7 @@
       <c r="AI65" s="3"/>
       <c r="AJ65" s="3"/>
     </row>
-    <row r="66" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="66" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -5091,7 +5091,7 @@
         <v>3.7499999999999999E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="67" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -5141,7 +5141,7 @@
       <c r="AI67" s="3"/>
       <c r="AJ67" s="3"/>
     </row>
-    <row r="68" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="68" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A68" s="3" t="str">
         <f t="shared" ref="A68:A131" si="29">A67</f>
         <v>Green</v>
@@ -5191,7 +5191,7 @@
       <c r="AI68" s="3"/>
       <c r="AJ68" s="3"/>
     </row>
-    <row r="69" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="69" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A69" s="3" t="str">
         <f t="shared" si="29"/>
         <v>Green</v>
@@ -5241,7 +5241,7 @@
       <c r="AI69" s="3"/>
       <c r="AJ69" s="3"/>
     </row>
-    <row r="70" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="70" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A70" s="3" t="str">
         <f t="shared" si="29"/>
         <v>Green</v>
@@ -5291,7 +5291,7 @@
       <c r="AI70" s="3"/>
       <c r="AJ70" s="3"/>
     </row>
-    <row r="71" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="71" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A71" s="3" t="str">
         <f t="shared" si="29"/>
         <v>Green</v>
@@ -5341,7 +5341,7 @@
       <c r="AI71" s="3"/>
       <c r="AJ71" s="3"/>
     </row>
-    <row r="72" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="72" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A72" s="3" t="str">
         <f t="shared" si="29"/>
         <v>Green</v>
@@ -5391,7 +5391,7 @@
       <c r="AI72" s="3"/>
       <c r="AJ72" s="3"/>
     </row>
-    <row r="73" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="73" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A73" s="3" t="str">
         <f t="shared" si="29"/>
         <v>Green</v>
@@ -5441,7 +5441,7 @@
       <c r="AI73" s="3"/>
       <c r="AJ73" s="3"/>
     </row>
-    <row r="74" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="74" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A74" s="3" t="str">
         <f t="shared" si="29"/>
         <v>Green</v>
@@ -5579,7 +5579,7 @@
         <v>4.027777777777778E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="75" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A75" s="3" t="str">
         <f t="shared" si="29"/>
         <v>Green</v>
@@ -5629,7 +5629,7 @@
       <c r="AI75" s="3"/>
       <c r="AJ75" s="3"/>
     </row>
-    <row r="76" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="76" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A76" s="3" t="str">
         <f t="shared" si="29"/>
         <v>Green</v>
@@ -5679,7 +5679,7 @@
       <c r="AI76" s="3"/>
       <c r="AJ76" s="3"/>
     </row>
-    <row r="77" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="77" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A77" s="3" t="str">
         <f t="shared" si="29"/>
         <v>Green</v>
@@ -5732,7 +5732,7 @@
       <c r="AI77" s="3"/>
       <c r="AJ77" s="3"/>
     </row>
-    <row r="78" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="78" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A78" s="3" t="str">
         <f t="shared" si="29"/>
         <v>Green</v>
@@ -5869,7 +5869,7 @@
         <v>4.2361111111111106E-2</v>
       </c>
     </row>
-    <row r="79" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="79" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A79" s="3" t="str">
         <f t="shared" si="29"/>
         <v>Green</v>
@@ -5919,7 +5919,7 @@
       <c r="AI79" s="3"/>
       <c r="AJ79" s="3"/>
     </row>
-    <row r="80" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="80" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A80" s="3" t="str">
         <f t="shared" si="29"/>
         <v>Green</v>
@@ -5969,7 +5969,7 @@
       <c r="AI80" s="3"/>
       <c r="AJ80" s="3"/>
     </row>
-    <row r="81" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="81" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A81" s="3" t="str">
         <f t="shared" si="29"/>
         <v>Green</v>
@@ -6019,7 +6019,7 @@
       <c r="AI81" s="3"/>
       <c r="AJ81" s="3"/>
     </row>
-    <row r="82" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="82" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A82" s="3" t="str">
         <f t="shared" si="29"/>
         <v>Green</v>
@@ -6069,7 +6069,7 @@
       <c r="AI82" s="3"/>
       <c r="AJ82" s="3"/>
     </row>
-    <row r="83" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="83" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A83" s="3" t="str">
         <f t="shared" si="29"/>
         <v>Green</v>
@@ -6119,7 +6119,7 @@
       <c r="AI83" s="3"/>
       <c r="AJ83" s="3"/>
     </row>
-    <row r="84" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="84" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A84" s="3" t="str">
         <f t="shared" si="29"/>
         <v>Green</v>
@@ -6169,7 +6169,7 @@
       <c r="AI84" s="3"/>
       <c r="AJ84" s="3"/>
     </row>
-    <row r="85" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="85" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A85" s="3" t="str">
         <f t="shared" si="29"/>
         <v>Green</v>
@@ -6219,7 +6219,7 @@
       <c r="AI85" s="3"/>
       <c r="AJ85" s="3"/>
     </row>
-    <row r="86" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="86" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A86" s="3" t="str">
         <f t="shared" si="29"/>
         <v>Green</v>
@@ -6269,7 +6269,7 @@
       <c r="AI86" s="3"/>
       <c r="AJ86" s="3"/>
     </row>
-    <row r="87" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="87" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A87" s="3" t="str">
         <f t="shared" si="29"/>
         <v>Green</v>
@@ -6322,7 +6322,7 @@
       <c r="AI87" s="3"/>
       <c r="AJ87" s="3"/>
     </row>
-    <row r="88" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="88" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A88" s="3" t="str">
         <f t="shared" si="29"/>
         <v>Green</v>
@@ -6372,7 +6372,7 @@
       <c r="AI88" s="3"/>
       <c r="AJ88" s="3"/>
     </row>
-    <row r="89" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="89" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A89" s="3" t="str">
         <f t="shared" si="29"/>
         <v>Green</v>
@@ -6510,7 +6510,7 @@
         <v>4.7222222222222221E-2</v>
       </c>
     </row>
-    <row r="90" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="90" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A90" s="3" t="str">
         <f t="shared" si="29"/>
         <v>Green</v>
@@ -6560,7 +6560,7 @@
       <c r="AI90" s="3"/>
       <c r="AJ90" s="3"/>
     </row>
-    <row r="91" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="91" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A91" s="3" t="str">
         <f t="shared" si="29"/>
         <v>Green</v>
@@ -6610,7 +6610,7 @@
       <c r="AI91" s="3"/>
       <c r="AJ91" s="3"/>
     </row>
-    <row r="92" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="92" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A92" s="3" t="str">
         <f t="shared" si="29"/>
         <v>Green</v>
@@ -6660,7 +6660,7 @@
       <c r="AI92" s="3"/>
       <c r="AJ92" s="3"/>
     </row>
-    <row r="93" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="93" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A93" s="3" t="str">
         <f t="shared" si="29"/>
         <v>Green</v>
@@ -6710,7 +6710,7 @@
       <c r="AI93" s="3"/>
       <c r="AJ93" s="3"/>
     </row>
-    <row r="94" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="94" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A94" s="3" t="str">
         <f t="shared" si="29"/>
         <v>Green</v>
@@ -6760,7 +6760,7 @@
       <c r="AI94" s="3"/>
       <c r="AJ94" s="3"/>
     </row>
-    <row r="95" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="95" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A95" s="3" t="str">
         <f t="shared" si="29"/>
         <v>Green</v>
@@ -6810,7 +6810,7 @@
       <c r="AI95" s="3"/>
       <c r="AJ95" s="3"/>
     </row>
-    <row r="96" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="96" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A96" s="3" t="str">
         <f t="shared" si="29"/>
         <v>Green</v>
@@ -6860,7 +6860,7 @@
       <c r="AI96" s="3"/>
       <c r="AJ96" s="3"/>
     </row>
-    <row r="97" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="97" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A97" s="3" t="str">
         <f t="shared" si="29"/>
         <v>Green</v>
@@ -6998,7 +6998,7 @@
         <v>4.9305555555555554E-2</v>
       </c>
     </row>
-    <row r="98" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="98" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A98" s="3" t="str">
         <f t="shared" si="29"/>
         <v>Green</v>
@@ -7048,7 +7048,7 @@
       <c r="AI98" s="3"/>
       <c r="AJ98" s="3"/>
     </row>
-    <row r="99" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="99" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A99" s="3" t="str">
         <f t="shared" si="29"/>
         <v>Green</v>
@@ -7098,7 +7098,7 @@
       <c r="AI99" s="3"/>
       <c r="AJ99" s="3"/>
     </row>
-    <row r="100" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="100" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A100" s="3" t="str">
         <f t="shared" si="29"/>
         <v>Green</v>
@@ -7148,7 +7148,7 @@
       <c r="AI100" s="3"/>
       <c r="AJ100" s="3"/>
     </row>
-    <row r="101" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="101" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A101" s="3" t="str">
         <f t="shared" si="29"/>
         <v>Green</v>
@@ -7198,7 +7198,7 @@
       <c r="AI101" s="3"/>
       <c r="AJ101" s="3"/>
     </row>
-    <row r="102" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="102" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A102" s="3" t="str">
         <f t="shared" si="29"/>
         <v>Green</v>
@@ -7248,7 +7248,7 @@
       <c r="AI102" s="3"/>
       <c r="AJ102" s="3"/>
     </row>
-    <row r="103" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="103" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A103" s="3" t="str">
         <f t="shared" si="29"/>
         <v>Green</v>
@@ -7298,7 +7298,7 @@
       <c r="AI103" s="3"/>
       <c r="AJ103" s="3"/>
     </row>
-    <row r="104" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="104" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A104" s="3" t="str">
         <f t="shared" si="29"/>
         <v>Green</v>
@@ -7348,7 +7348,7 @@
       <c r="AI104" s="3"/>
       <c r="AJ104" s="3"/>
     </row>
-    <row r="105" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="105" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A105" s="3" t="str">
         <f t="shared" si="29"/>
         <v>Green</v>
@@ -7398,7 +7398,7 @@
       <c r="AI105" s="3"/>
       <c r="AJ105" s="3"/>
     </row>
-    <row r="106" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="106" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A106" s="3" t="str">
         <f t="shared" si="29"/>
         <v>Green</v>
@@ -7537,7 +7537,7 @@
         <v>5.2083333333333329E-2</v>
       </c>
     </row>
-    <row r="107" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="107" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A107" s="3" t="str">
         <f t="shared" si="29"/>
         <v>Green</v>
@@ -7587,7 +7587,7 @@
       <c r="AI107" s="3"/>
       <c r="AJ107" s="3"/>
     </row>
-    <row r="108" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="108" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A108" s="3" t="str">
         <f t="shared" si="29"/>
         <v>Green</v>
@@ -7637,7 +7637,7 @@
       <c r="AI108" s="3"/>
       <c r="AJ108" s="3"/>
     </row>
-    <row r="109" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="109" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A109" s="3" t="str">
         <f t="shared" si="29"/>
         <v>Green</v>
@@ -7687,7 +7687,7 @@
       <c r="AI109" s="3"/>
       <c r="AJ109" s="3"/>
     </row>
-    <row r="110" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="110" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A110" s="3" t="str">
         <f t="shared" si="29"/>
         <v>Green</v>
@@ -7737,7 +7737,7 @@
       <c r="AI110" s="3"/>
       <c r="AJ110" s="3"/>
     </row>
-    <row r="111" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="111" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A111" s="3" t="str">
         <f t="shared" si="29"/>
         <v>Green</v>
@@ -7787,7 +7787,7 @@
       <c r="AI111" s="3"/>
       <c r="AJ111" s="3"/>
     </row>
-    <row r="112" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="112" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A112" s="3" t="str">
         <f t="shared" si="29"/>
         <v>Green</v>
@@ -7837,7 +7837,7 @@
       <c r="AI112" s="3"/>
       <c r="AJ112" s="3"/>
     </row>
-    <row r="113" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="113" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A113" s="3" t="str">
         <f t="shared" si="29"/>
         <v>Green</v>
@@ -7887,7 +7887,7 @@
       <c r="AI113" s="3"/>
       <c r="AJ113" s="3"/>
     </row>
-    <row r="114" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="114" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A114" s="3" t="str">
         <f t="shared" si="29"/>
         <v>Green</v>
@@ -7987,7 +7987,7 @@
         <v>5.4166666666666662E-2</v>
       </c>
     </row>
-    <row r="115" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="115" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A115" s="3" t="str">
         <f t="shared" si="29"/>
         <v>Green</v>
@@ -8076,7 +8076,7 @@
       <c r="AI115" s="3"/>
       <c r="AJ115" s="3"/>
     </row>
-    <row r="116" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="116" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A116" s="3" t="str">
         <f t="shared" si="29"/>
         <v>Green</v>
@@ -8126,7 +8126,7 @@
       <c r="AI116" s="3"/>
       <c r="AJ116" s="3"/>
     </row>
-    <row r="117" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="117" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A117" s="3" t="str">
         <f t="shared" si="29"/>
         <v>Green</v>
@@ -8176,7 +8176,7 @@
       <c r="AI117" s="3"/>
       <c r="AJ117" s="3"/>
     </row>
-    <row r="118" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="118" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A118" s="3" t="str">
         <f t="shared" si="29"/>
         <v>Green</v>
@@ -8226,7 +8226,7 @@
       <c r="AI118" s="3"/>
       <c r="AJ118" s="3"/>
     </row>
-    <row r="119" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="119" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A119" s="3" t="str">
         <f t="shared" si="29"/>
         <v>Green</v>
@@ -8276,7 +8276,7 @@
       <c r="AI119" s="3"/>
       <c r="AJ119" s="3"/>
     </row>
-    <row r="120" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="120" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A120" s="3" t="str">
         <f t="shared" si="29"/>
         <v>Green</v>
@@ -8326,7 +8326,7 @@
       <c r="AI120" s="3"/>
       <c r="AJ120" s="3"/>
     </row>
-    <row r="121" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="121" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A121" s="3" t="str">
         <f t="shared" si="29"/>
         <v>Green</v>
@@ -8376,7 +8376,7 @@
       <c r="AI121" s="3"/>
       <c r="AJ121" s="3"/>
     </row>
-    <row r="122" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="122" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A122" s="3" t="str">
         <f t="shared" si="29"/>
         <v>Green</v>
@@ -8426,7 +8426,7 @@
       <c r="AI122" s="3"/>
       <c r="AJ122" s="3"/>
     </row>
-    <row r="123" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="123" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A123" s="3" t="str">
         <f t="shared" si="29"/>
         <v>Green</v>
@@ -8479,7 +8479,7 @@
       <c r="AI123" s="3"/>
       <c r="AJ123" s="3"/>
     </row>
-    <row r="124" spans="1:41" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="124" spans="1:41" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A124" s="3" t="str">
         <f t="shared" si="29"/>
         <v>Green</v>
@@ -8617,7 +8617,7 @@
         <v>5.6249999999999994E-2</v>
       </c>
     </row>
-    <row r="125" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="125" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A125" s="3" t="str">
         <f t="shared" si="29"/>
         <v>Green</v>
@@ -8670,7 +8670,7 @@
       <c r="AI125" s="3"/>
       <c r="AJ125" s="3"/>
     </row>
-    <row r="126" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="126" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A126" s="3" t="str">
         <f t="shared" si="29"/>
         <v>Green</v>
@@ -8723,7 +8723,7 @@
       <c r="AI126" s="3"/>
       <c r="AJ126" s="3"/>
     </row>
-    <row r="127" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="127" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A127" s="3" t="str">
         <f t="shared" si="29"/>
         <v>Green</v>
@@ -8776,7 +8776,7 @@
       <c r="AI127" s="3"/>
       <c r="AJ127" s="3"/>
     </row>
-    <row r="128" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="128" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A128" s="3" t="str">
         <f t="shared" si="29"/>
         <v>Green</v>
@@ -8829,7 +8829,7 @@
       <c r="AI128" s="3"/>
       <c r="AJ128" s="3"/>
     </row>
-    <row r="129" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="129" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A129" s="3" t="str">
         <f t="shared" si="29"/>
         <v>Green</v>
@@ -8882,7 +8882,7 @@
       <c r="AI129" s="3"/>
       <c r="AJ129" s="3"/>
     </row>
-    <row r="130" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="130" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A130" s="3" t="str">
         <f t="shared" si="29"/>
         <v>Green</v>
@@ -8935,7 +8935,7 @@
       <c r="AI130" s="3"/>
       <c r="AJ130" s="3"/>
     </row>
-    <row r="131" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="131" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A131" s="3" t="str">
         <f t="shared" si="29"/>
         <v>Green</v>
@@ -8988,7 +8988,7 @@
       <c r="AI131" s="3"/>
       <c r="AJ131" s="3"/>
     </row>
-    <row r="132" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="132" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A132" s="3" t="str">
         <f t="shared" ref="A132:A151" si="50">A131</f>
         <v>Green</v>
@@ -9041,7 +9041,7 @@
       <c r="AI132" s="3"/>
       <c r="AJ132" s="3"/>
     </row>
-    <row r="133" spans="1:41" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="133" spans="1:41" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A133" s="3" t="str">
         <f t="shared" si="50"/>
         <v>Green</v>
@@ -9179,7 +9179,7 @@
         <v>5.8333333333333327E-2</v>
       </c>
     </row>
-    <row r="134" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="134" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A134" s="3" t="str">
         <f t="shared" si="50"/>
         <v>Green</v>
@@ -9232,7 +9232,7 @@
       <c r="AI134" s="3"/>
       <c r="AJ134" s="3"/>
     </row>
-    <row r="135" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="135" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A135" s="3" t="str">
         <f t="shared" si="50"/>
         <v>Green</v>
@@ -9285,7 +9285,7 @@
       <c r="AI135" s="3"/>
       <c r="AJ135" s="3"/>
     </row>
-    <row r="136" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="136" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A136" s="3" t="str">
         <f t="shared" si="50"/>
         <v>Green</v>
@@ -9338,7 +9338,7 @@
       <c r="AI136" s="3"/>
       <c r="AJ136" s="3"/>
     </row>
-    <row r="137" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="137" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A137" s="3" t="str">
         <f t="shared" si="50"/>
         <v>Green</v>
@@ -9391,7 +9391,7 @@
       <c r="AI137" s="3"/>
       <c r="AJ137" s="3"/>
     </row>
-    <row r="138" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="138" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A138" s="3" t="str">
         <f t="shared" si="50"/>
         <v>Green</v>
@@ -9444,7 +9444,7 @@
       <c r="AI138" s="3"/>
       <c r="AJ138" s="3"/>
     </row>
-    <row r="139" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="139" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A139" s="3" t="str">
         <f t="shared" si="50"/>
         <v>Green</v>
@@ -9497,7 +9497,7 @@
       <c r="AI139" s="3"/>
       <c r="AJ139" s="3"/>
     </row>
-    <row r="140" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="140" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A140" s="3" t="str">
         <f t="shared" si="50"/>
         <v>Green</v>
@@ -9550,7 +9550,7 @@
       <c r="AI140" s="3"/>
       <c r="AJ140" s="3"/>
     </row>
-    <row r="141" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="141" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A141" s="3" t="str">
         <f t="shared" si="50"/>
         <v>Green</v>
@@ -9603,7 +9603,7 @@
       <c r="AI141" s="3"/>
       <c r="AJ141" s="3"/>
     </row>
-    <row r="142" spans="1:41" x14ac:dyDescent="0.5">
+    <row r="142" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A142" s="3" t="str">
         <f t="shared" si="50"/>
         <v>Green</v>
@@ -9741,7 +9741,7 @@
         <v>8.1250000000000058E-2</v>
       </c>
     </row>
-    <row r="143" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
+    <row r="143" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
       <c r="A143" s="3" t="str">
         <f t="shared" si="50"/>
         <v>Green</v>
@@ -9793,7 +9793,7 @@
       <c r="AH143" s="3"/>
       <c r="AI143" s="3"/>
     </row>
-    <row r="144" spans="1:41" hidden="1" x14ac:dyDescent="0.5">
+    <row r="144" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
       <c r="A144" s="3" t="str">
         <f t="shared" si="50"/>
         <v>Green</v>
@@ -9845,7 +9845,7 @@
       <c r="AH144" s="3"/>
       <c r="AI144" s="3"/>
     </row>
-    <row r="145" spans="1:35" hidden="1" x14ac:dyDescent="0.5">
+    <row r="145" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A145" s="3" t="str">
         <f t="shared" si="50"/>
         <v>Green</v>
@@ -9894,7 +9894,7 @@
       <c r="AH145" s="3"/>
       <c r="AI145" s="3"/>
     </row>
-    <row r="146" spans="1:35" hidden="1" x14ac:dyDescent="0.5">
+    <row r="146" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A146" s="3" t="str">
         <f t="shared" si="50"/>
         <v>Green</v>
@@ -9943,7 +9943,7 @@
       <c r="AH146" s="3"/>
       <c r="AI146" s="3"/>
     </row>
-    <row r="147" spans="1:35" hidden="1" x14ac:dyDescent="0.5">
+    <row r="147" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A147" s="3" t="str">
         <f t="shared" si="50"/>
         <v>Green</v>
@@ -9992,7 +9992,7 @@
       <c r="AH147" s="3"/>
       <c r="AI147" s="3"/>
     </row>
-    <row r="148" spans="1:35" hidden="1" x14ac:dyDescent="0.5">
+    <row r="148" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A148" s="3" t="str">
         <f t="shared" si="50"/>
         <v>Green</v>
@@ -10041,7 +10041,7 @@
       <c r="AH148" s="3"/>
       <c r="AI148" s="3"/>
     </row>
-    <row r="149" spans="1:35" hidden="1" x14ac:dyDescent="0.5">
+    <row r="149" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A149" s="3" t="str">
         <f t="shared" si="50"/>
         <v>Green</v>
@@ -10090,7 +10090,7 @@
       <c r="AH149" s="3"/>
       <c r="AI149" s="3"/>
     </row>
-    <row r="150" spans="1:35" hidden="1" x14ac:dyDescent="0.5">
+    <row r="150" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A150" s="3" t="str">
         <f t="shared" si="50"/>
         <v>Green</v>
@@ -10139,7 +10139,7 @@
       <c r="AH150" s="3"/>
       <c r="AI150" s="3"/>
     </row>
-    <row r="151" spans="1:35" hidden="1" x14ac:dyDescent="0.5">
+    <row r="151" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A151" s="3" t="str">
         <f t="shared" si="50"/>
         <v>Green</v>
@@ -10188,73 +10188,73 @@
       <c r="AH151" s="3"/>
       <c r="AI151" s="3"/>
     </row>
-    <row r="152" spans="1:35" x14ac:dyDescent="0.5">
+    <row r="152" spans="1:35" x14ac:dyDescent="0.3">
       <c r="AF152" s="3"/>
       <c r="AG152" s="3"/>
       <c r="AH152" s="3"/>
       <c r="AI152" s="3"/>
     </row>
-    <row r="153" spans="1:35" x14ac:dyDescent="0.5">
+    <row r="153" spans="1:35" x14ac:dyDescent="0.3">
       <c r="AF153" s="3"/>
       <c r="AG153" s="3"/>
       <c r="AH153" s="3"/>
       <c r="AI153" s="3"/>
     </row>
-    <row r="154" spans="1:35" x14ac:dyDescent="0.5">
+    <row r="154" spans="1:35" x14ac:dyDescent="0.3">
       <c r="AF154" s="3"/>
       <c r="AG154" s="3"/>
       <c r="AH154" s="3"/>
       <c r="AI154" s="3"/>
     </row>
-    <row r="155" spans="1:35" x14ac:dyDescent="0.5">
+    <row r="155" spans="1:35" x14ac:dyDescent="0.3">
       <c r="AF155" s="3"/>
       <c r="AG155" s="3"/>
       <c r="AH155" s="3"/>
       <c r="AI155" s="3"/>
     </row>
-    <row r="156" spans="1:35" x14ac:dyDescent="0.5">
+    <row r="156" spans="1:35" x14ac:dyDescent="0.3">
       <c r="AF156" s="3"/>
       <c r="AG156" s="3"/>
       <c r="AH156" s="3"/>
       <c r="AI156" s="3"/>
     </row>
-    <row r="157" spans="1:35" x14ac:dyDescent="0.5">
+    <row r="157" spans="1:35" x14ac:dyDescent="0.3">
       <c r="AF157" s="3"/>
       <c r="AG157" s="3"/>
       <c r="AH157" s="3"/>
       <c r="AI157" s="3"/>
     </row>
-    <row r="158" spans="1:35" x14ac:dyDescent="0.5">
+    <row r="158" spans="1:35" x14ac:dyDescent="0.3">
       <c r="AF158" s="3"/>
       <c r="AG158" s="3"/>
       <c r="AH158" s="3"/>
       <c r="AI158" s="3"/>
     </row>
-    <row r="159" spans="1:35" x14ac:dyDescent="0.5">
+    <row r="159" spans="1:35" x14ac:dyDescent="0.3">
       <c r="AF159" s="3"/>
       <c r="AG159" s="3"/>
       <c r="AH159" s="3"/>
       <c r="AI159" s="3"/>
     </row>
-    <row r="160" spans="1:35" x14ac:dyDescent="0.5">
+    <row r="160" spans="1:35" x14ac:dyDescent="0.3">
       <c r="AF160" s="3"/>
       <c r="AG160" s="3"/>
       <c r="AH160" s="3"/>
       <c r="AI160" s="3"/>
     </row>
-    <row r="161" spans="32:35" x14ac:dyDescent="0.5">
+    <row r="161" spans="32:35" x14ac:dyDescent="0.3">
       <c r="AF161" s="3"/>
       <c r="AG161" s="3"/>
       <c r="AH161" s="3"/>
       <c r="AI161" s="3"/>
     </row>
-    <row r="162" spans="32:35" x14ac:dyDescent="0.5">
+    <row r="162" spans="32:35" x14ac:dyDescent="0.3">
       <c r="AF162" s="3"/>
       <c r="AG162" s="3"/>
       <c r="AH162" s="3"/>
       <c r="AI162" s="3"/>
     </row>
-    <row r="163" spans="32:35" x14ac:dyDescent="0.5">
+    <row r="163" spans="32:35" x14ac:dyDescent="0.3">
       <c r="AF163" s="3"/>
       <c r="AG163" s="3"/>
       <c r="AH163" s="3"/>
@@ -10269,23 +10269,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E1DDA1C-7AF6-47B0-9CCF-ACDF9A5FF277}">
   <dimension ref="A1:Q163"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="S5" sqref="S5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.796875" style="3"/>
-    <col min="2" max="2" width="12.796875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="8.46484375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="8.77734375" style="3"/>
+    <col min="2" max="2" width="12.77734375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="8.44140625" style="3" customWidth="1"/>
     <col min="4" max="4" width="43" style="3" customWidth="1"/>
-    <col min="5" max="9" width="10.73046875" style="22" customWidth="1"/>
-    <col min="10" max="14" width="8.796875" style="3"/>
-    <col min="15" max="15" width="4.46484375" style="1" customWidth="1"/>
-    <col min="16" max="16384" width="8.796875" style="1"/>
+    <col min="5" max="9" width="10.77734375" style="22" customWidth="1"/>
+    <col min="10" max="14" width="8.77734375" style="3"/>
+    <col min="15" max="15" width="4.44140625" style="1" customWidth="1"/>
+    <col min="16" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="37.9" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:17" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -10333,7 +10333,7 @@
       </c>
       <c r="Q1" s="20"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>81</v>
       </c>
@@ -10383,7 +10383,7 @@
         <v>1.8749999999999999E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="str">
         <f>A2</f>
         <v>Red</v>
@@ -10395,7 +10395,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="str">
         <f t="shared" ref="A4:A67" si="1">A3</f>
         <v>Red</v>
@@ -10412,7 +10412,7 @@
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -10429,7 +10429,7 @@
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -10446,7 +10446,7 @@
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -10463,7 +10463,7 @@
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -10517,7 +10517,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -10534,7 +10534,7 @@
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -10554,7 +10554,7 @@
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -10571,7 +10571,7 @@
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -10591,7 +10591,7 @@
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -10608,7 +10608,7 @@
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -10625,7 +10625,7 @@
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -10642,7 +10642,7 @@
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -10662,7 +10662,7 @@
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -10716,7 +10716,7 @@
         <v>2.4305555555555552E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -10733,7 +10733,7 @@
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -10750,7 +10750,7 @@
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -10767,7 +10767,7 @@
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -10784,7 +10784,7 @@
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -10838,7 +10838,7 @@
         <v>2.7083333333333331E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -10850,7 +10850,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -10867,7 +10867,7 @@
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -10887,7 +10887,7 @@
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -10941,7 +10941,7 @@
         <v>2.9861111111111109E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -10961,7 +10961,7 @@
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -10981,7 +10981,7 @@
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -11001,7 +11001,7 @@
       <c r="H29" s="3"/>
       <c r="I29" s="3"/>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -11021,7 +11021,7 @@
       <c r="H30" s="3"/>
       <c r="I30" s="3"/>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -11041,7 +11041,7 @@
       <c r="H31" s="3"/>
       <c r="I31" s="3"/>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -11056,7 +11056,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -11076,7 +11076,7 @@
       <c r="H33" s="3"/>
       <c r="I33" s="3"/>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -11096,7 +11096,7 @@
       <c r="H34" s="3"/>
       <c r="I34" s="3"/>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -11116,7 +11116,7 @@
       <c r="H35" s="3"/>
       <c r="I35" s="3"/>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -11170,7 +11170,7 @@
         <v>3.1944444444444442E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -11190,7 +11190,7 @@
       <c r="H37" s="3"/>
       <c r="I37" s="3"/>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="str">
         <f>A34</f>
         <v>Red</v>
@@ -11210,7 +11210,7 @@
       <c r="H38" s="3"/>
       <c r="I38" s="3"/>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -11230,7 +11230,7 @@
       <c r="H39" s="3"/>
       <c r="I39" s="3"/>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -11245,7 +11245,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -11265,7 +11265,7 @@
       <c r="H41" s="3"/>
       <c r="I41" s="3"/>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -11285,7 +11285,7 @@
       <c r="H42" s="3"/>
       <c r="I42" s="3"/>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -11305,7 +11305,7 @@
       <c r="H43" s="3"/>
       <c r="I43" s="3"/>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -11325,7 +11325,7 @@
       <c r="H44" s="3"/>
       <c r="I44" s="3"/>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -11345,7 +11345,7 @@
       <c r="H45" s="3"/>
       <c r="I45" s="3"/>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -11399,7 +11399,7 @@
         <v>3.3333333333333333E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -11419,7 +11419,7 @@
       <c r="H47" s="3"/>
       <c r="I47" s="3"/>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -11439,7 +11439,7 @@
       <c r="H48" s="3"/>
       <c r="I48" s="3"/>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -11493,7 +11493,7 @@
         <v>3.5416666666666666E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -11510,7 +11510,7 @@
       <c r="H50" s="3"/>
       <c r="I50" s="3"/>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -11527,7 +11527,7 @@
       <c r="H51" s="3"/>
       <c r="I51" s="3"/>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -11544,7 +11544,7 @@
       <c r="H52" s="3"/>
       <c r="I52" s="3"/>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -11564,7 +11564,7 @@
       <c r="H53" s="3"/>
       <c r="I53" s="3"/>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -11581,7 +11581,7 @@
       <c r="H54" s="3"/>
       <c r="I54" s="3"/>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -11598,7 +11598,7 @@
       <c r="H55" s="3"/>
       <c r="I55" s="3"/>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -11615,7 +11615,7 @@
       <c r="H56" s="3"/>
       <c r="I56" s="3"/>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -11632,7 +11632,7 @@
       <c r="H57" s="3"/>
       <c r="I57" s="3"/>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -11644,7 +11644,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -11661,7 +11661,7 @@
       <c r="H59" s="3"/>
       <c r="I59" s="3"/>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -11678,7 +11678,7 @@
       <c r="H60" s="3"/>
       <c r="I60" s="3"/>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -11732,7 +11732,7 @@
         <v>3.7499999999999999E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A62" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -11749,7 +11749,7 @@
       <c r="H62" s="3"/>
       <c r="I62" s="3"/>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -11766,7 +11766,7 @@
       <c r="H63" s="3"/>
       <c r="I63" s="3"/>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A64" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -11783,7 +11783,7 @@
       <c r="H64" s="3"/>
       <c r="I64" s="3"/>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -11800,7 +11800,7 @@
       <c r="H65" s="3"/>
       <c r="I65" s="3"/>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -11812,7 +11812,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -11829,7 +11829,7 @@
       <c r="H67" s="3"/>
       <c r="I67" s="3"/>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68" s="3" t="str">
         <f t="shared" ref="A68:A131" si="10">A67</f>
         <v>Red</v>
@@ -11849,7 +11849,7 @@
       <c r="H68" s="3"/>
       <c r="I68" s="3"/>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69" s="3" t="str">
         <f t="shared" si="10"/>
         <v>Red</v>
@@ -11869,7 +11869,7 @@
       <c r="H69" s="3"/>
       <c r="I69" s="3"/>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" s="3" t="str">
         <f t="shared" si="10"/>
         <v>Red</v>
@@ -11889,7 +11889,7 @@
       <c r="H70" s="3"/>
       <c r="I70" s="3"/>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71" s="3" t="str">
         <f t="shared" si="10"/>
         <v>Red</v>
@@ -11909,7 +11909,7 @@
       <c r="H71" s="3"/>
       <c r="I71" s="3"/>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72" s="3" t="str">
         <f t="shared" si="10"/>
         <v>Red</v>
@@ -11929,7 +11929,7 @@
       <c r="H72" s="3"/>
       <c r="I72" s="3"/>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73" s="3" t="str">
         <f t="shared" si="10"/>
         <v>Red</v>
@@ -11949,7 +11949,7 @@
       <c r="H73" s="3"/>
       <c r="I73" s="3"/>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74" s="3" t="str">
         <f t="shared" si="10"/>
         <v>Red</v>
@@ -11969,7 +11969,7 @@
       <c r="H74" s="3"/>
       <c r="I74" s="3"/>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75" s="3" t="str">
         <f t="shared" si="10"/>
         <v>Red</v>
@@ -11989,7 +11989,7 @@
       <c r="H75" s="3"/>
       <c r="I75" s="3"/>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76" s="3" t="str">
         <f t="shared" si="10"/>
         <v>Red</v>
@@ -12009,7 +12009,7 @@
       <c r="H76" s="3"/>
       <c r="I76" s="3"/>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77" s="3" t="str">
         <f t="shared" si="10"/>
         <v>Red</v>
@@ -12029,7 +12029,7 @@
       <c r="H77" s="3"/>
       <c r="I77" s="3"/>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A78" s="3" t="s">
         <v>98</v>
       </c>
@@ -12040,7 +12040,7 @@
       <c r="H78" s="3"/>
       <c r="I78" s="3"/>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79" s="3" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
@@ -12052,7 +12052,7 @@
       <c r="H79" s="3"/>
       <c r="I79" s="3"/>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A80" s="3" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
@@ -12064,7 +12064,7 @@
       <c r="H80" s="3"/>
       <c r="I80" s="3"/>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A81" s="3" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
@@ -12076,7 +12076,7 @@
       <c r="H81" s="3"/>
       <c r="I81" s="3"/>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A82" s="3" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
@@ -12088,7 +12088,7 @@
       <c r="H82" s="3"/>
       <c r="I82" s="3"/>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A83" s="3" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
@@ -12100,7 +12100,7 @@
       <c r="H83" s="3"/>
       <c r="I83" s="3"/>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A84" s="3" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
@@ -12112,7 +12112,7 @@
       <c r="H84" s="3"/>
       <c r="I84" s="3"/>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A85" s="3" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
@@ -12124,7 +12124,7 @@
       <c r="H85" s="3"/>
       <c r="I85" s="3"/>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A86" s="3" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
@@ -12136,7 +12136,7 @@
       <c r="H86" s="3"/>
       <c r="I86" s="3"/>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A87" s="3" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
@@ -12148,7 +12148,7 @@
       <c r="H87" s="3"/>
       <c r="I87" s="3"/>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A88" s="3" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
@@ -12160,7 +12160,7 @@
       <c r="H88" s="3"/>
       <c r="I88" s="3"/>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A89" s="3" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
@@ -12172,7 +12172,7 @@
       <c r="H89" s="3"/>
       <c r="I89" s="3"/>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A90" s="3" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
@@ -12184,7 +12184,7 @@
       <c r="H90" s="3"/>
       <c r="I90" s="3"/>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A91" s="3" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
@@ -12196,7 +12196,7 @@
       <c r="H91" s="3"/>
       <c r="I91" s="3"/>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A92" s="3" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
@@ -12208,7 +12208,7 @@
       <c r="H92" s="3"/>
       <c r="I92" s="3"/>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A93" s="3" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
@@ -12220,7 +12220,7 @@
       <c r="H93" s="3"/>
       <c r="I93" s="3"/>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A94" s="3" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
@@ -12232,7 +12232,7 @@
       <c r="H94" s="3"/>
       <c r="I94" s="3"/>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A95" s="3" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
@@ -12244,7 +12244,7 @@
       <c r="H95" s="3"/>
       <c r="I95" s="3"/>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A96" s="3" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
@@ -12256,7 +12256,7 @@
       <c r="H96" s="3"/>
       <c r="I96" s="3"/>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A97" s="3" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
@@ -12268,7 +12268,7 @@
       <c r="H97" s="3"/>
       <c r="I97" s="3"/>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A98" s="3" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
@@ -12280,7 +12280,7 @@
       <c r="H98" s="3"/>
       <c r="I98" s="3"/>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A99" s="3" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
@@ -12292,7 +12292,7 @@
       <c r="H99" s="3"/>
       <c r="I99" s="3"/>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A100" s="3" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
@@ -12304,7 +12304,7 @@
       <c r="H100" s="3"/>
       <c r="I100" s="3"/>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A101" s="3" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
@@ -12316,7 +12316,7 @@
       <c r="H101" s="3"/>
       <c r="I101" s="3"/>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A102" s="3" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
@@ -12328,7 +12328,7 @@
       <c r="H102" s="3"/>
       <c r="I102" s="3"/>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A103" s="3" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
@@ -12340,7 +12340,7 @@
       <c r="H103" s="3"/>
       <c r="I103" s="3"/>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A104" s="3" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
@@ -12352,7 +12352,7 @@
       <c r="H104" s="3"/>
       <c r="I104" s="3"/>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A105" s="3" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
@@ -12364,7 +12364,7 @@
       <c r="H105" s="3"/>
       <c r="I105" s="3"/>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A106" s="3" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
@@ -12376,7 +12376,7 @@
       <c r="H106" s="3"/>
       <c r="I106" s="3"/>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A107" s="3" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
@@ -12388,7 +12388,7 @@
       <c r="H107" s="3"/>
       <c r="I107" s="3"/>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A108" s="3" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
@@ -12400,7 +12400,7 @@
       <c r="H108" s="3"/>
       <c r="I108" s="3"/>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A109" s="3" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
@@ -12412,7 +12412,7 @@
       <c r="H109" s="3"/>
       <c r="I109" s="3"/>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A110" s="3" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
@@ -12424,7 +12424,7 @@
       <c r="H110" s="3"/>
       <c r="I110" s="3"/>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A111" s="3" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
@@ -12436,7 +12436,7 @@
       <c r="H111" s="3"/>
       <c r="I111" s="3"/>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A112" s="3" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
@@ -12448,7 +12448,7 @@
       <c r="H112" s="3"/>
       <c r="I112" s="3"/>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A113" s="3" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
@@ -12460,7 +12460,7 @@
       <c r="H113" s="3"/>
       <c r="I113" s="3"/>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A114" s="3" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
@@ -12472,7 +12472,7 @@
       <c r="H114" s="3"/>
       <c r="I114" s="3"/>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A115" s="3" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
@@ -12484,7 +12484,7 @@
       <c r="H115" s="3"/>
       <c r="I115" s="3"/>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A116" s="3" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
@@ -12496,7 +12496,7 @@
       <c r="H116" s="3"/>
       <c r="I116" s="3"/>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A117" s="3" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
@@ -12508,7 +12508,7 @@
       <c r="H117" s="3"/>
       <c r="I117" s="3"/>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A118" s="3" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
@@ -12520,7 +12520,7 @@
       <c r="H118" s="3"/>
       <c r="I118" s="3"/>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A119" s="3" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
@@ -12532,7 +12532,7 @@
       <c r="H119" s="3"/>
       <c r="I119" s="3"/>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A120" s="3" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
@@ -12544,7 +12544,7 @@
       <c r="H120" s="3"/>
       <c r="I120" s="3"/>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A121" s="3" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
@@ -12556,7 +12556,7 @@
       <c r="H121" s="3"/>
       <c r="I121" s="3"/>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A122" s="3" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
@@ -12568,7 +12568,7 @@
       <c r="H122" s="3"/>
       <c r="I122" s="3"/>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A123" s="3" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
@@ -12580,7 +12580,7 @@
       <c r="H123" s="3"/>
       <c r="I123" s="3"/>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A124" s="3" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
@@ -12592,7 +12592,7 @@
       <c r="H124" s="3"/>
       <c r="I124" s="3"/>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A125" s="3" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
@@ -12604,7 +12604,7 @@
       <c r="H125" s="3"/>
       <c r="I125" s="3"/>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A126" s="3" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
@@ -12616,7 +12616,7 @@
       <c r="H126" s="3"/>
       <c r="I126" s="3"/>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A127" s="3" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
@@ -12628,7 +12628,7 @@
       <c r="H127" s="3"/>
       <c r="I127" s="3"/>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A128" s="3" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
@@ -12640,7 +12640,7 @@
       <c r="H128" s="3"/>
       <c r="I128" s="3"/>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A129" s="3" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
@@ -12652,7 +12652,7 @@
       <c r="H129" s="3"/>
       <c r="I129" s="3"/>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A130" s="3" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
@@ -12664,7 +12664,7 @@
       <c r="H130" s="3"/>
       <c r="I130" s="3"/>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A131" s="3" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
@@ -12676,7 +12676,7 @@
       <c r="H131" s="3"/>
       <c r="I131" s="3"/>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A132" s="3" t="str">
         <f t="shared" ref="A132:A154" si="11">A131</f>
         <v xml:space="preserve"> </v>
@@ -12688,7 +12688,7 @@
       <c r="H132" s="3"/>
       <c r="I132" s="3"/>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A133" s="3" t="str">
         <f t="shared" si="11"/>
         <v xml:space="preserve"> </v>
@@ -12700,7 +12700,7 @@
       <c r="H133" s="3"/>
       <c r="I133" s="3"/>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A134" s="3" t="str">
         <f t="shared" si="11"/>
         <v xml:space="preserve"> </v>
@@ -12712,7 +12712,7 @@
       <c r="H134" s="3"/>
       <c r="I134" s="3"/>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A135" s="3" t="str">
         <f t="shared" si="11"/>
         <v xml:space="preserve"> </v>
@@ -12724,7 +12724,7 @@
       <c r="H135" s="3"/>
       <c r="I135" s="3"/>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A136" s="3" t="str">
         <f t="shared" si="11"/>
         <v xml:space="preserve"> </v>
@@ -12736,7 +12736,7 @@
       <c r="H136" s="3"/>
       <c r="I136" s="3"/>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A137" s="3" t="str">
         <f t="shared" si="11"/>
         <v xml:space="preserve"> </v>
@@ -12748,7 +12748,7 @@
       <c r="H137" s="3"/>
       <c r="I137" s="3"/>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A138" s="3" t="str">
         <f t="shared" si="11"/>
         <v xml:space="preserve"> </v>
@@ -12760,7 +12760,7 @@
       <c r="H138" s="3"/>
       <c r="I138" s="3"/>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A139" s="3" t="str">
         <f t="shared" si="11"/>
         <v xml:space="preserve"> </v>
@@ -12772,7 +12772,7 @@
       <c r="H139" s="3"/>
       <c r="I139" s="3"/>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A140" s="3" t="str">
         <f t="shared" si="11"/>
         <v xml:space="preserve"> </v>
@@ -12784,7 +12784,7 @@
       <c r="H140" s="3"/>
       <c r="I140" s="3"/>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A141" s="3" t="str">
         <f t="shared" si="11"/>
         <v xml:space="preserve"> </v>
@@ -12796,7 +12796,7 @@
       <c r="H141" s="3"/>
       <c r="I141" s="3"/>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A142" s="3" t="str">
         <f t="shared" si="11"/>
         <v xml:space="preserve"> </v>
@@ -12808,7 +12808,7 @@
       <c r="H142" s="3"/>
       <c r="I142" s="3"/>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A143" s="3" t="str">
         <f t="shared" si="11"/>
         <v xml:space="preserve"> </v>
@@ -12820,7 +12820,7 @@
       <c r="H143" s="3"/>
       <c r="I143" s="3"/>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A144" s="3" t="str">
         <f t="shared" si="11"/>
         <v xml:space="preserve"> </v>
@@ -12832,7 +12832,7 @@
       <c r="H144" s="3"/>
       <c r="I144" s="3"/>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A145" s="3" t="str">
         <f t="shared" si="11"/>
         <v xml:space="preserve"> </v>
@@ -12844,7 +12844,7 @@
       <c r="H145" s="3"/>
       <c r="I145" s="3"/>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A146" s="3" t="str">
         <f t="shared" si="11"/>
         <v xml:space="preserve"> </v>
@@ -12856,7 +12856,7 @@
       <c r="H146" s="3"/>
       <c r="I146" s="3"/>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A147" s="3" t="str">
         <f t="shared" si="11"/>
         <v xml:space="preserve"> </v>
@@ -12867,7 +12867,7 @@
       <c r="G147" s="3"/>
       <c r="H147" s="3"/>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A148" s="3" t="str">
         <f t="shared" si="11"/>
         <v xml:space="preserve"> </v>
@@ -12878,7 +12878,7 @@
       <c r="G148" s="3"/>
       <c r="H148" s="3"/>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A149" s="3" t="str">
         <f t="shared" si="11"/>
         <v xml:space="preserve"> </v>
@@ -12889,7 +12889,7 @@
       <c r="G149" s="3"/>
       <c r="H149" s="3"/>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A150" s="3" t="str">
         <f t="shared" si="11"/>
         <v xml:space="preserve"> </v>
@@ -12900,7 +12900,7 @@
       <c r="G150" s="3"/>
       <c r="H150" s="3"/>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A151" s="3" t="str">
         <f t="shared" si="11"/>
         <v xml:space="preserve"> </v>
@@ -12911,7 +12911,7 @@
       <c r="G151" s="3"/>
       <c r="H151" s="3"/>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A152" s="3" t="str">
         <f t="shared" si="11"/>
         <v xml:space="preserve"> </v>
@@ -12922,7 +12922,7 @@
       <c r="G152" s="3"/>
       <c r="H152" s="3"/>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A153" s="3" t="str">
         <f t="shared" si="11"/>
         <v xml:space="preserve"> </v>
@@ -12933,7 +12933,7 @@
       <c r="G153" s="3"/>
       <c r="H153" s="3"/>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A154" s="3" t="str">
         <f t="shared" si="11"/>
         <v xml:space="preserve"> </v>
@@ -12944,55 +12944,55 @@
       <c r="G154" s="3"/>
       <c r="H154" s="3"/>
     </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E155" s="3"/>
       <c r="F155" s="3"/>
       <c r="G155" s="3"/>
       <c r="H155" s="3"/>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E156" s="3"/>
       <c r="F156" s="3"/>
       <c r="G156" s="3"/>
       <c r="H156" s="3"/>
     </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E157" s="3"/>
       <c r="F157" s="3"/>
       <c r="G157" s="3"/>
       <c r="H157" s="3"/>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E158" s="3"/>
       <c r="F158" s="3"/>
       <c r="G158" s="3"/>
       <c r="H158" s="3"/>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E159" s="3"/>
       <c r="F159" s="3"/>
       <c r="G159" s="3"/>
       <c r="H159" s="3"/>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E160" s="3"/>
       <c r="F160" s="3"/>
       <c r="G160" s="3"/>
       <c r="H160" s="3"/>
     </row>
-    <row r="161" spans="5:8" x14ac:dyDescent="0.5">
+    <row r="161" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E161" s="3"/>
       <c r="F161" s="3"/>
       <c r="G161" s="3"/>
       <c r="H161" s="3"/>
     </row>
-    <row r="162" spans="5:8" x14ac:dyDescent="0.5">
+    <row r="162" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E162" s="3"/>
       <c r="F162" s="3"/>
       <c r="G162" s="3"/>
       <c r="H162" s="3"/>
     </row>
-    <row r="163" spans="5:8" x14ac:dyDescent="0.5">
+    <row r="163" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E163" s="3"/>
       <c r="F163" s="3"/>
       <c r="G163" s="3"/>

</xml_diff>